<commit_message>
working on smooth wing movement
</commit_message>
<xml_diff>
--- a/Tower B-40 DevLog.xlsx
+++ b/Tower B-40 DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HB_Laboratories\Unity\Games\Tower_B-40\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E285B79-FF10-4BFF-8404-677B1CC21ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0B2654-B18A-4BBC-8550-4963F53FEE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="11170" xr2:uid="{D4A67F96-856A-41A8-9F6B-49CFA39147C8}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{D4A67F96-856A-41A8-9F6B-49CFA39147C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Tower B-40</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Movement function over input, animation handler</t>
+  </si>
+  <si>
+    <t>I should do the todo tasks.</t>
+  </si>
+  <si>
+    <t>Added acceleration animation for smoother movement, working on wings movement</t>
   </si>
 </sst>
 </file>
@@ -507,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2298B5DB-E3B3-42A3-9333-97CF41039696}">
   <dimension ref="B1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -612,7 +618,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="6">
+        <v>44986</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="11" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Camera&Eyes script, movement fix
</commit_message>
<xml_diff>
--- a/Tower B-40 DevLog.xlsx
+++ b/Tower B-40 DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HB_Laboratories\Unity\Games\Tower_B-40\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5672B6-5347-463D-B727-54EC14B031B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5693B54-650A-47EA-AEAB-FC071C9294B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="20430" windowHeight="11170" xr2:uid="{D4A67F96-856A-41A8-9F6B-49CFA39147C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D4A67F96-856A-41A8-9F6B-49CFA39147C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Tower B-40</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>fuck</t>
+  </si>
+  <si>
+    <t>Actually fix the damn movement script, Camera system from FB2020</t>
+  </si>
+  <si>
+    <t>Actually fixed the damn movement script, camera aiming system, eye movements</t>
   </si>
 </sst>
 </file>
@@ -114,29 +120,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Bahnschrift SemiBold Condensed"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="리디바탕"/>
       <family val="2"/>
+      <charset val="129"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="리디바탕"/>
       <family val="2"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="리디바탕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Agency FB"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -149,7 +158,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,30 +193,30 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,158 +534,168 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2298B5DB-E3B3-42A3-9333-97CF41039696}">
   <dimension ref="B1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="8.7265625" style="2" customWidth="1"/>
-    <col min="3" max="8" width="8.7265625" style="2"/>
-    <col min="9" max="9" width="8.7265625" style="8"/>
-    <col min="10" max="10" width="31" style="7" customWidth="1"/>
-    <col min="11" max="11" width="28.6328125" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="8.7265625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="8.7265625" style="1"/>
+    <col min="9" max="9" width="8.7265625" style="7"/>
+    <col min="10" max="10" width="31" style="6" customWidth="1"/>
+    <col min="11" max="11" width="28.6328125" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" ht="27" x14ac:dyDescent="0.5">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I6" s="4" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H7" s="2" t="s">
+    <row r="7" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>41334</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H8" s="2" t="s">
+    <row r="8" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>42430</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="2" t="s">
+    <row r="9" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>44256</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I10" s="6">
+    <row r="10" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="5">
         <v>44986</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H11" s="2" t="s">
+    <row r="11" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>11018</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I12" s="6">
+    <row r="12" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="5">
         <v>11383</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="44" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="5">
+        <v>46478</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:11" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="44" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>